<commit_message>
Feedback from industry visits week#7
Here we go team, I forsee these coming in handy down the line!
</commit_message>
<xml_diff>
--- a/Game Feedback.xlsx
+++ b/Game Feedback.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>No.</t>
   </si>
@@ -113,6 +113,96 @@
   </si>
   <si>
     <t>Art style is good, but the level is not that interesting, because for now we don't have enemies to attack you and in game we don't know how to pass the level(no goal).The most frustrating thing is I can't kill the enemy in testing level.(Kiki)</t>
+  </si>
+  <si>
+    <t>Need a breadcrumb system to help player from getting lost (Frank Arnot-StormCloud)</t>
+  </si>
+  <si>
+    <t>Player should be able to see and predict the consequence of their actions clearly, e.g project future platform location (Frank Arnot-StormCloud)</t>
+  </si>
+  <si>
+    <t>Platforming elements felt good, but level could have more space (bumping head in confined areas) (Frank Arnot-StormCloud)</t>
+  </si>
+  <si>
+    <t>Scripted Events sucg as dialogue will help provide context for player, such as what their goal is (Frank Arnot-StormCloud)</t>
+  </si>
+  <si>
+    <t>Potentially have change in audio que when Raven on platform with coresponding plane, not when the change happens, so as to communicate to the player what the result will be? (Us)</t>
+  </si>
+  <si>
+    <t>We kind of Want the player to get lost? The challenge will be making being lost fun (Us)</t>
+  </si>
+  <si>
+    <t>Maybe retain chiptune instrumentation in the soundtrack, but supplement with organic instrumentation evocative of the tropes assigned to each plane (Us)</t>
+  </si>
+  <si>
+    <t>If we get this to work it will be brilliant, the concept is there, we just need to ensure we communicate with the player enough (Frank Arnot-StormCloud)</t>
+  </si>
+  <si>
+    <t>Summarising, that we need to improve Visual Grammer (Audio can help with this too) (Frank Arnot-StormCloud)</t>
+  </si>
+  <si>
+    <t>Believes it will be fun, as solving puzzles is always satisfying, long as the player doesn’t become too frustrated to complete. (Frank Arnot-StormCloud)</t>
+  </si>
+  <si>
+    <t>Game will go down well as long as its clear what player's goal is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We're in a good place for Week#7 </t>
+  </si>
+  <si>
+    <t>Keep it simple, we have a product at the moment, we just need to improve upon it (Graham &amp; Ricardo - Outplay)</t>
+  </si>
+  <si>
+    <t>Should we wish to discuss game further, or starting up our own company and taking the game further he is open to meet up with us for coffee and a chat (David Hamilton - Ninja Kiwi)</t>
+  </si>
+  <si>
+    <t>Have something to highlight when player is near somehting they can interact with(David Hamilton - Ninja Kiwi)  e.g  an outline lighting up around the Lever?</t>
+  </si>
+  <si>
+    <t>If the game lacks a way for the player to make early progress then they might not get a chance to experience the really great parts of the game, have these elements sooner? (David Hamilton - Ninja Kiwi)</t>
+  </si>
+  <si>
+    <t>Should we have some kind of hint system should the player take too long to progress? Need to not hold player's hand too much though (David Hamilton - Ninja Kiwi)</t>
+  </si>
+  <si>
+    <t>We will only need this one level for the vertical slice (David Hamilton - Ninja Kiwi)</t>
+  </si>
+  <si>
+    <t>Begin work on the tutorial elements sooner rather than later, they may feel like a low priority task, but they are deceivingly difficult to do well and time-intensive (David Hamilton - Ninja Kiwi)</t>
+  </si>
+  <si>
+    <t>Requires some form of 'Soft-tutorial' to guide player at first, and then leave them to it, otherwise they may become frustrated before getting any enjoyment (David Hamilton - Ninja Kiwi)</t>
+  </si>
+  <si>
+    <t>Is the Veil jump a fundamental aspect of the game? Is it necessary? What does it add? (Graham &amp; Ricardo - Outplay)</t>
+  </si>
+  <si>
+    <t>Awesome Music! (Graham - Outplay)</t>
+  </si>
+  <si>
+    <t>Does the frustration of veiljump detract from what is already good? The puzzle solving? (Graham &amp; Ricardo - Outplay)</t>
+  </si>
+  <si>
+    <t>If we include too many 'skill' elements in our game they detract from our puzzle elements and we isolate a smaller demographic (Graham &amp; Ricardo - Outplay)</t>
+  </si>
+  <si>
+    <t>Similar to Megaman, in that each section is its own unique puzzle, but needs to avoid frustrating player (Graham &amp; Ricardo - Outplay)</t>
+  </si>
+  <si>
+    <t>We need to find a balance between opposing puzzle and skill elements (Graham &amp; Ricardo - Outplay)</t>
+  </si>
+  <si>
+    <t>Avoid any timing pressures which could be frustrating (Graham &amp; Ricardo - Outplay)</t>
+  </si>
+  <si>
+    <t>Likes the concept for each plane's visual art-style - tropish (Graham &amp; Ricardo - Outplay)</t>
+  </si>
+  <si>
+    <t>If we are going to keep Veil Jump then we need to introduce it as a mechanic to player early on and make it worth keeping (Graham &amp; Ricardo - Outplay)</t>
+  </si>
+  <si>
+    <t>Will require much visual and audible cues to communicate with the player their progress, also, should there be a checkpoint system of some kind? (Graham &amp; Ricardo - Outplay)</t>
   </si>
 </sst>
 </file>
@@ -180,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -207,6 +297,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,6 +1011,336 @@
       </c>
       <c r="C20" s="7">
         <v>43391</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>20</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>28</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>30</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>31</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>36</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>37</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>38</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="7">
+        <v>43398</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>39</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>40</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>41</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>42</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>43</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>45</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>46</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>47</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>48</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="7">
+        <v>43399</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>49</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="7">
+        <v>43399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>